<commit_message>
add tooltips for all creates
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -29,7 +29,7 @@
     <t>ESTADO ACTUAL</t>
   </si>
   <si>
-    <t>2024-10-01T03:00:00.000Z</t>
+    <t>2024-09-01T10:30:00.000Z</t>
   </si>
   <si>
     <t>NOMBRE DEL PRODUCTO</t>
@@ -47,10 +47,10 @@
     <t>SUBTOTAL</t>
   </si>
   <si>
-    <t>holabro</t>
-  </si>
-  <si>
-    <t>23</t>
+    <t>nguwevoertsdsdfsdfdsnuev</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
   <si>
     <t>ml</t>
@@ -59,25 +59,10 @@
     <t>500</t>
   </si>
   <si>
-    <t>holabrodcsdfdsfs</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>GR</t>
-  </si>
-  <si>
-    <t>nguwevoertsdsdfsdfdsnuev</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
     <t>holabro2</t>
   </si>
   <si>
-    <t>231</t>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -501,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +516,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="5" width="30" customWidth="1"/>
@@ -568,7 +553,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>11500</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -579,47 +564,13 @@
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="3">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2">
-        <v>117500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3">
-        <v>115500</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tooltips for edit usuario, inventario, producto, pedido, perfil and proveedor
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,65 +4,86 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Pedido" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="Producto" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Inventarios" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
   <si>
-    <t>NÚMERO</t>
-  </si>
-  <si>
-    <t>FECHA DEL PEDIDO</t>
-  </si>
-  <si>
-    <t>pendiente</t>
-  </si>
-  <si>
-    <t>ESTADO ACTUAL</t>
-  </si>
-  <si>
-    <t>2024-09-01T10:30:00.000Z</t>
-  </si>
-  <si>
-    <t>NOMBRE DEL PRODUCTO</t>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t>Cerveza artesanal de alta calidad</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>Artesanal</t>
+  </si>
+  <si>
+    <t>CONTENIDO</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>UNIDAD DE MEDIDA</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>Alcohólico</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>CATEGORÍA</t>
+  </si>
+  <si>
+    <t>Cerveza</t>
   </si>
   <si>
     <t>CANTIDAD</t>
   </si>
   <si>
-    <t>UNIDAD DE MEDIDA</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>SUBTOTAL</t>
-  </si>
-  <si>
-    <t>nguwevoertsdsdfsdfdsnuev</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>holabro2</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>MÁXIMO STOCK</t>
+  </si>
+  <si>
+    <t>FECHA DE ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>asdasdasdsa</t>
+  </si>
+  <si>
+    <t>2024-10-07T20:29:04.937Z</t>
+  </si>
+  <si>
+    <t>?test</t>
+  </si>
+  <si>
+    <t>2024-10-15T00:03:30.008Z</t>
   </si>
 </sst>
 </file>
@@ -468,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -485,24 +506,64 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -516,61 +577,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="5" width="30" customWidth="1"/>
+    <col min="1" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>569</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5555</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20000</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3">
-        <v>5000</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add confirm in update or create usuario, inventario, producto, pedido, perfil or proveedor
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -5,14 +5,13 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Producto" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Inventarios" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -20,31 +19,31 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>Cerveza Artesanal</t>
+    <t>NuevoTestdfgfdg</t>
   </si>
   <si>
     <t>DESCRIPCIÓN</t>
   </si>
   <si>
-    <t>Cerveza artesanal de alta calidad</t>
+    <t>sdfsdfdsfsd</t>
   </si>
   <si>
     <t>MARCA</t>
   </si>
   <si>
-    <t>Artesanal</t>
+    <t>carozzigterg</t>
   </si>
   <si>
     <t>CONTENIDO</t>
   </si>
   <si>
-    <t>50</t>
+    <t>500</t>
   </si>
   <si>
     <t>UNIDAD DE MEDIDA</t>
   </si>
   <si>
-    <t>L</t>
+    <t>GR</t>
   </si>
   <si>
     <t>TIPO</t>
@@ -56,34 +55,10 @@
     <t>PRECIO</t>
   </si>
   <si>
-    <t>1500</t>
-  </si>
-  <si>
     <t>CATEGORÍA</t>
   </si>
   <si>
-    <t>Cerveza</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>MÁXIMO STOCK</t>
-  </si>
-  <si>
-    <t>FECHA DE ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>asdasdasdsa</t>
-  </si>
-  <si>
-    <t>2024-10-07T20:29:04.937Z</t>
-  </si>
-  <si>
-    <t>?test</t>
-  </si>
-  <si>
-    <t>2024-10-15T00:03:30.008Z</t>
+    <t>Gaseosa</t>
   </si>
 </sst>
 </file>
@@ -555,15 +530,15 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -573,60 +548,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="4" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2">
-        <v>569</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3">
-        <v>5555</v>
-      </c>
-      <c r="C3" s="3">
-        <v>20000</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add validations for null usuarios, inventarios, productos, pedidos or proveedores
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -19,25 +19,25 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>NuevoTestdfgfdg</t>
+    <t>Cerveza Artesanal Actualizada test</t>
   </si>
   <si>
     <t>DESCRIPCIÓN</t>
   </si>
   <si>
-    <t>sdfsdfdsfsd</t>
+    <t>testttasdasd</t>
   </si>
   <si>
     <t>MARCA</t>
   </si>
   <si>
-    <t>carozzigterg</t>
+    <t>carozzitest</t>
   </si>
   <si>
     <t>CONTENIDO</t>
   </si>
   <si>
-    <t>500</t>
+    <t>400</t>
   </si>
   <si>
     <t>UNIDAD DE MEDIDA</t>
@@ -55,10 +55,13 @@
     <t>PRECIO</t>
   </si>
   <si>
+    <t>NO REGISTRADO</t>
+  </si>
+  <si>
     <t>CATEGORÍA</t>
   </si>
   <si>
-    <t>Gaseosa</t>
+    <t>Vino</t>
   </si>
 </sst>
 </file>
@@ -530,15 +533,15 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update git ignore for secret files
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,64 +4,211 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Producto" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>CARACTERISTICAS GENERALES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>Cerveza Artesanal Actualizada test</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN</t>
-  </si>
-  <si>
-    <t>testttasdasd</t>
-  </si>
-  <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>carozzitest</t>
-  </si>
-  <si>
-    <t>CONTENIDO</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>UNIDAD DE MEDIDA</t>
-  </si>
-  <si>
-    <t>GR</t>
-  </si>
-  <si>
-    <t>TIPO</t>
-  </si>
-  <si>
-    <t>Alcohólico</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>NO REGISTRADO</t>
-  </si>
-  <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
-    <t>Vino</t>
+    <t>RUT</t>
+  </si>
+  <si>
+    <t>CORREO ELECTRÓNICO</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>REGISTRO</t>
+  </si>
+  <si>
+    <t>Ignacio Munoz</t>
+  </si>
+  <si>
+    <t>50.232.225-2</t>
+  </si>
+  <si>
+    <t>ignacio.munoz2001@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>14/09/2024</t>
+  </si>
+  <si>
+    <t>Alexander Carrasco</t>
+  </si>
+  <si>
+    <t>20.630.735-8</t>
+  </si>
+  <si>
+    <t>alexander.carrasco2101@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>20.630.725-8</t>
+  </si>
+  <si>
+    <t>ialeczander@gmail.com</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>20.555.444-5</t>
+  </si>
+  <si>
+    <t>adwemin@alumnos.ubiobio.com</t>
+  </si>
+  <si>
+    <t>26/09/2024</t>
+  </si>
+  <si>
+    <t>Alexander Test</t>
+  </si>
+  <si>
+    <t>12.222.333-5</t>
+  </si>
+  <si>
+    <t>nuevoTasdest@gmail.com</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>12.345.678-9</t>
+  </si>
+  <si>
+    <t>bsantaelena590@gmail.com</t>
+  </si>
+  <si>
+    <t>Alexander Nuevo Test</t>
+  </si>
+  <si>
+    <t>20.630.333-8</t>
+  </si>
+  <si>
+    <t>nuevoTGest@gmail.com</t>
+  </si>
+  <si>
+    <t>Estudent</t>
+  </si>
+  <si>
+    <t>07/10/2024</t>
+  </si>
+  <si>
+    <t>holabro</t>
+  </si>
+  <si>
+    <t>20.333.222-5</t>
+  </si>
+  <si>
+    <t>nuevotesdadst@gmail.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>19/10/2024</t>
+  </si>
+  <si>
+    <t>Alexander Nuevo</t>
+  </si>
+  <si>
+    <t>22.222.333-5</t>
+  </si>
+  <si>
+    <t>addsfasdasd@gmail.com</t>
+  </si>
+  <si>
+    <t>2333333-5</t>
+  </si>
+  <si>
+    <t>fsdfdfsdfdsdf@gmail.com</t>
+  </si>
+  <si>
+    <t>21/10/2024</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>20630735-5</t>
+  </si>
+  <si>
+    <t>administradasdasdr@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>20630735-2</t>
+  </si>
+  <si>
+    <t>adminisaasdsatrador@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>asdsdaasddas</t>
+  </si>
+  <si>
+    <t>20.333222-5</t>
+  </si>
+  <si>
+    <t>administrqwqweador@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>12312312-3</t>
+  </si>
+  <si>
+    <t>ewfwasdasdefw@gmail.com</t>
+  </si>
+  <si>
+    <t>2222222-4</t>
+  </si>
+  <si>
+    <t>adawdasdsamin@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>12.222333-k</t>
+  </si>
+  <si>
+    <t>adminassdaistrador@alumnos.ubiobio.cl</t>
+  </si>
+  <si>
+    <t>asdsadsaasddsasad</t>
+  </si>
+  <si>
+    <t>2222222-5</t>
+  </si>
+  <si>
+    <t>ialeczanasdder@gmail.com</t>
+  </si>
+  <si>
+    <t>Tomas Bawssy</t>
+  </si>
+  <si>
+    <t>12.222.333-7</t>
+  </si>
+  <si>
+    <t>tomaxlion@gmail.com</t>
+  </si>
+  <si>
+    <t>24/10/2024</t>
+  </si>
+  <si>
+    <t>12.222.333-2</t>
+  </si>
+  <si>
+    <t>basdadas@gmail.com</t>
+  </si>
+  <si>
+    <t>27/10/2024</t>
   </si>
 </sst>
 </file>
@@ -467,87 +614,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update home screen with add new container for notifications and refactory stetic for stats
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,58 +4,49 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Usuario" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>CONTENIDO</t>
-  </si>
-  <si>
-    <t>UNIDAD DE MEDIDA</t>
-  </si>
-  <si>
-    <t>Cerveza Artesanal Actualizada test</t>
-  </si>
-  <si>
-    <t>No registrado</t>
-  </si>
-  <si>
-    <t>Cerveza</t>
-  </si>
-  <si>
-    <t>holabronuevotest</t>
-  </si>
-  <si>
-    <t>picopalkelee</t>
-  </si>
-  <si>
-    <t>Gaseosa</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>GR</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>CARACTERISTICAS GENERALES</t>
+  </si>
+  <si>
+    <t>RUT</t>
+  </si>
+  <si>
+    <t>12.222.333-2</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>basdadas@gmail.com</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>NOMBRE COMPLETO</t>
+  </si>
+  <si>
+    <t>Tomas Bawssy</t>
+  </si>
+  <si>
+    <t>FECHA DE REGISTRO</t>
+  </si>
+  <si>
+    <t>27/10/2024</t>
+  </si>
+  <si>
+    <t>ÚLTIMA ACTUALIZACIÓN</t>
   </si>
 </sst>
 </file>
@@ -461,77 +452,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:B7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
add export unique object for table
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,49 +4,125 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Usuario" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Inventario" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
   <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>12.222.333-2</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>basdadas@gmail.com</t>
-  </si>
-  <si>
-    <t>ROL</t>
-  </si>
-  <si>
-    <t>Administrador</t>
-  </si>
-  <si>
-    <t>NOMBRE COMPLETO</t>
-  </si>
-  <si>
-    <t>Tomas Bawssy</t>
-  </si>
-  <si>
-    <t>FECHA DE REGISTRO</t>
-  </si>
-  <si>
-    <t>27/10/2024</t>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>Patio trasero</t>
+  </si>
+  <si>
+    <t>MÁXIMO STOCK</t>
   </si>
   <si>
     <t>ÚLTIMA ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>28/10/2024</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL PRODUCTO</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t>CATEGORÍA</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal Actualizada test</t>
+  </si>
+  <si>
+    <t>NO REGISTRADO</t>
+  </si>
+  <si>
+    <t>holabrofdssdtest</t>
+  </si>
+  <si>
+    <t>Cerveza</t>
+  </si>
+  <si>
+    <t>Sin Alcohol</t>
+  </si>
+  <si>
+    <t>holabro2dfsad3</t>
+  </si>
+  <si>
+    <t>testttasdasd</t>
+  </si>
+  <si>
+    <t>Vino</t>
+  </si>
+  <si>
+    <t>Ron 2 test</t>
+  </si>
+  <si>
+    <t>asasfafasfsafsfasasffasasfda</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Alcohólico</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>Nuevo Vodka Vegano</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>nuevo test 2</t>
+  </si>
+  <si>
+    <t>Agua mineral</t>
+  </si>
+  <si>
+    <t>NuevoTest25</t>
+  </si>
+  <si>
+    <t>Cigarrillo</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal Actualizada tesasdasdt</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal Actualizada testasdasd</t>
+  </si>
+  <si>
+    <t>Néctar</t>
+  </si>
+  <si>
+    <t>testqwrwqd</t>
+  </si>
+  <si>
+    <t>Ron Vodka cualificado por admins</t>
   </si>
 </sst>
 </file>
@@ -452,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -477,40 +553,16 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+      <c r="B3" s="3">
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -520,4 +572,218 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="6" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add value precio in pedido_producto and implement this function in frontend and backend
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -26,10 +26,13 @@
     <t>MÁXIMO STOCK</t>
   </si>
   <si>
-    <t>ÚLTIMA ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>28/10/2024</t>
+    <t>STOCK ACTUAL</t>
+  </si>
+  <si>
+    <t>FECHA DE ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>2024-10-28T19:46:07.904Z</t>
   </si>
   <si>
     <t>NOMBRE DEL PRODUCTO</t>
@@ -50,73 +53,67 @@
     <t>CANTIDAD</t>
   </si>
   <si>
+    <t>NuevoTest25</t>
+  </si>
+  <si>
+    <t>NO REGISTRADO</t>
+  </si>
+  <si>
+    <t>holabrofdssdtest</t>
+  </si>
+  <si>
+    <t>Cigarrillo</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal Actualizada testasdasd</t>
+  </si>
+  <si>
+    <t>Néctar</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal Actualizada tesasdasdt</t>
+  </si>
+  <si>
+    <t>testttasdasd</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>nuevo test 2</t>
+  </si>
+  <si>
+    <t>Agua mineral</t>
+  </si>
+  <si>
+    <t>Sin Alcohol</t>
+  </si>
+  <si>
+    <t>Ron 2 test</t>
+  </si>
+  <si>
+    <t>asasfafasfsafsfasasffasasfda</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Alcohólico</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>Nuevo Vodka Vegano</t>
+  </si>
+  <si>
     <t>Cerveza Artesanal Actualizada test</t>
   </si>
   <si>
-    <t>NO REGISTRADO</t>
-  </si>
-  <si>
-    <t>holabrofdssdtest</t>
-  </si>
-  <si>
     <t>Cerveza</t>
-  </si>
-  <si>
-    <t>Sin Alcohol</t>
-  </si>
-  <si>
-    <t>holabro2dfsad3</t>
-  </si>
-  <si>
-    <t>testttasdasd</t>
-  </si>
-  <si>
-    <t>Vino</t>
-  </si>
-  <si>
-    <t>Ron 2 test</t>
-  </si>
-  <si>
-    <t>asasfafasfsafsfasasffasasfda</t>
-  </si>
-  <si>
-    <t>Ron</t>
-  </si>
-  <si>
-    <t>Alcohólico</t>
-  </si>
-  <si>
-    <t>Vodka</t>
-  </si>
-  <si>
-    <t>Nuevo Vodka Vegano</t>
-  </si>
-  <si>
-    <t>Otro</t>
-  </si>
-  <si>
-    <t>nuevo test 2</t>
-  </si>
-  <si>
-    <t>Agua mineral</t>
-  </si>
-  <si>
-    <t>NuevoTest25</t>
-  </si>
-  <si>
-    <t>Cigarrillo</t>
-  </si>
-  <si>
-    <t>Cerveza Artesanal Actualizada tesasdasdt</t>
-  </si>
-  <si>
-    <t>Snack</t>
-  </si>
-  <si>
-    <t>Cerveza Artesanal Actualizada testasdasd</t>
-  </si>
-  <si>
-    <t>Néctar</t>
   </si>
   <si>
     <t>testqwrwqd</t>
@@ -528,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -561,8 +558,16 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +581,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="30" customWidth="1"/>
@@ -584,62 +589,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -647,7 +652,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>21</v>
@@ -656,129 +661,109 @@
         <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2">
         <v>23</v>
-      </c>
-      <c r="F4" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F9" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create and implement secundary table
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Inventario" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Pedido" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -12,114 +12,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
   <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>Patio trasero</t>
-  </si>
-  <si>
-    <t>MÁXIMO STOCK</t>
-  </si>
-  <si>
-    <t>STOCK ACTUAL</t>
-  </si>
-  <si>
-    <t>FECHA DE ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>2024-10-28T19:46:07.904Z</t>
+    <t>NÚMERO</t>
+  </si>
+  <si>
+    <t>FECHA DEL PEDIDO</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>ESTADO ACTUAL</t>
+  </si>
+  <si>
+    <t>2024-09-01T10:30:00.000Z</t>
+  </si>
+  <si>
+    <t>TOTAL DEL PEDIDO</t>
+  </si>
+  <si>
+    <t>$105000</t>
   </si>
   <si>
     <t>NOMBRE DEL PRODUCTO</t>
   </si>
   <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN</t>
-  </si>
-  <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
-    <t>TIPO</t>
-  </si>
-  <si>
     <t>CANTIDAD</t>
   </si>
   <si>
-    <t>NuevoTest25</t>
-  </si>
-  <si>
-    <t>NO REGISTRADO</t>
-  </si>
-  <si>
-    <t>holabrofdssdtest</t>
-  </si>
-  <si>
-    <t>Cigarrillo</t>
-  </si>
-  <si>
-    <t>Otro</t>
-  </si>
-  <si>
-    <t>Cerveza Artesanal Actualizada testasdasd</t>
-  </si>
-  <si>
-    <t>Néctar</t>
-  </si>
-  <si>
-    <t>Cerveza Artesanal Actualizada tesasdasdt</t>
-  </si>
-  <si>
-    <t>testttasdasd</t>
-  </si>
-  <si>
-    <t>Snack</t>
-  </si>
-  <si>
-    <t>nuevo test 2</t>
-  </si>
-  <si>
-    <t>Agua mineral</t>
-  </si>
-  <si>
-    <t>Sin Alcohol</t>
-  </si>
-  <si>
-    <t>Ron 2 test</t>
-  </si>
-  <si>
-    <t>asasfafasfsafsfasasffasasfda</t>
-  </si>
-  <si>
-    <t>Ron</t>
-  </si>
-  <si>
-    <t>Alcohólico</t>
-  </si>
-  <si>
-    <t>Vodka</t>
-  </si>
-  <si>
-    <t>Nuevo Vodka Vegano</t>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
   </si>
   <si>
     <t>Cerveza Artesanal Actualizada test</t>
   </si>
   <si>
-    <t>Cerveza</t>
-  </si>
-  <si>
-    <t>testqwrwqd</t>
-  </si>
-  <si>
-    <t>Ron Vodka cualificado por admins</t>
+    <t>200</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>holabronuevotest</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -542,32 +485,32 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+      <c r="B2" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>173</v>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -581,190 +524,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="30" customWidth="1"/>
+    <col min="1" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3">
-        <v>3</v>
+      <c r="D3" s="3">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add validation in create and update producto inventario with calculate new stock post event
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,65 +4,34 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Pedido" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="Inventario" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
   <si>
-    <t>NÚMERO</t>
-  </si>
-  <si>
-    <t>FECHA DEL PEDIDO</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>ESTADO ACTUAL</t>
-  </si>
-  <si>
-    <t>2024-09-01T10:30:00.000Z</t>
-  </si>
-  <si>
-    <t>TOTAL DEL PEDIDO</t>
-  </si>
-  <si>
-    <t>$105000</t>
-  </si>
-  <si>
-    <t>NOMBRE DEL PRODUCTO</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>SUBTOTAL</t>
-  </si>
-  <si>
-    <t>Cerveza Artesanal Actualizada test</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>holabronuevotest</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>Patio Trasero</t>
+  </si>
+  <si>
+    <t>STOCK ACTUAL</t>
+  </si>
+  <si>
+    <t>MÁXIMO STOCK</t>
+  </si>
+  <si>
+    <t>FECHA DE ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>2024-11-21T20:44:55.948Z</t>
   </si>
 </sst>
 </file>
@@ -485,32 +454,32 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+      <c r="B4" s="2">
+        <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -520,60 +489,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="4" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add validations for productoInventario entity
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,34 +4,46 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Inventario" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>CARACTERISTICAS GENERALES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>NOMBRE</t>
   </si>
   <si>
+    <t>STOCK ACTUAL</t>
+  </si>
+  <si>
+    <t>MÁXIMO STOCK</t>
+  </si>
+  <si>
+    <t>ÚLTIMA ACTUALIZACIÓN</t>
+  </si>
+  <si>
     <t>Patio Trasero</t>
   </si>
   <si>
-    <t>STOCK ACTUAL</t>
-  </si>
-  <si>
-    <t>MÁXIMO STOCK</t>
-  </si>
-  <si>
-    <t>FECHA DE ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>2024-11-21T20:44:55.948Z</t>
+    <t>21/11/2024</t>
+  </si>
+  <si>
+    <t>No registrado</t>
+  </si>
+  <si>
+    <t>22/11/2024</t>
+  </si>
+  <si>
+    <t>asdfsdfs</t>
+  </si>
+  <si>
+    <t>Inventario Secundario</t>
+  </si>
+  <si>
+    <t>Inventario Principal</t>
   </si>
 </sst>
 </file>
@@ -437,55 +449,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>535</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>824</v>
+      </c>
+      <c r="C3" s="3">
+        <v>500</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>535</v>
+      </c>
+      <c r="C7" s="3">
+        <v>600</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>500</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix update pedido in service and validations
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,46 +4,65 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Pedido" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>STOCK ACTUAL</t>
-  </si>
-  <si>
-    <t>MÁXIMO STOCK</t>
-  </si>
-  <si>
-    <t>ÚLTIMA ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>Patio Trasero</t>
-  </si>
-  <si>
-    <t>21/11/2024</t>
-  </si>
-  <si>
-    <t>No registrado</t>
-  </si>
-  <si>
-    <t>22/11/2024</t>
-  </si>
-  <si>
-    <t>asdfsdfs</t>
-  </si>
-  <si>
-    <t>Inventario Secundario</t>
-  </si>
-  <si>
-    <t>Inventario Principal</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+  <si>
+    <t>CARACTERISTICAS GENERALES</t>
+  </si>
+  <si>
+    <t>NÚMERO</t>
+  </si>
+  <si>
+    <t>ESTADO ACTUAL</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>FECHA DEL PEDIDO</t>
+  </si>
+  <si>
+    <t>19/09/2024</t>
+  </si>
+  <si>
+    <t>TOTAL DEL PEDIDO</t>
+  </si>
+  <si>
+    <t>$105000</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL PRODUCTO</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Cerveza Artesanal Actualizada</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -449,124 +468,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
-        <v>535</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3000</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
-        <v>824</v>
-      </c>
-      <c r="C3" s="3">
-        <v>500</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>535</v>
-      </c>
-      <c r="C7" s="3">
-        <v>600</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>500</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reset password for create usuario
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,49 +4,46 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Usuario" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>CARACTERISTICAS GENERALES</t>
-  </si>
-  <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>20.630.735-8</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>ialeczander@gmail.com</t>
-  </si>
-  <si>
-    <t>ROL</t>
-  </si>
-  <si>
-    <t>Empleado</t>
-  </si>
-  <si>
-    <t>NOMBRE COMPLETO</t>
-  </si>
-  <si>
-    <t>Alexander Carrasco</t>
-  </si>
-  <si>
-    <t>FECHA DE REGISTRO</t>
-  </si>
-  <si>
-    <t>05/12/2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>STOCK ACTUAL</t>
+  </si>
+  <si>
+    <t>MÁXIMO STOCK</t>
   </si>
   <si>
     <t>ÚLTIMA ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>asdfsdfs</t>
+  </si>
+  <si>
+    <t>22/11/2024</t>
+  </si>
+  <si>
+    <t>Inventario Principal</t>
+  </si>
+  <si>
+    <t>Inventario Secundario</t>
+  </si>
+  <si>
+    <t>27/11/2024</t>
+  </si>
+  <si>
+    <t>Patio</t>
+  </si>
+  <si>
+    <t>asdd</t>
   </si>
 </sst>
 </file>
@@ -452,71 +449,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>155</v>
+      </c>
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>500</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="2">
+        <v>535</v>
+      </c>
+      <c r="C6" s="2">
+        <v>600</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="3">
+        <v>355</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1400</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
+      <c r="B8" s="2">
+        <v>406</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update alerts for error in productoinventario
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,46 +4,64 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Producto" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>CARACTERISTICAS GENERALES</t>
+  </si>
   <si>
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>STOCK ACTUAL</t>
-  </si>
-  <si>
-    <t>MÁXIMO STOCK</t>
-  </si>
-  <si>
-    <t>ÚLTIMA ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>asdfsdfs</t>
-  </si>
-  <si>
-    <t>22/11/2024</t>
-  </si>
-  <si>
-    <t>Inventario Principal</t>
-  </si>
-  <si>
-    <t>Inventario Secundario</t>
-  </si>
-  <si>
-    <t>27/11/2024</t>
-  </si>
-  <si>
-    <t>Patio</t>
-  </si>
-  <si>
-    <t>asdd</t>
+    <t>Cerveza Artesanal Actualizada</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t>Cerveza artesanal de alta calidad, edición limitada</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>Artesanal Premium</t>
+  </si>
+  <si>
+    <t>CONTENIDO</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>UNIDAD DE MEDIDA</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>bebida</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>CATEGORÍA</t>
+  </si>
+  <si>
+    <t>Bebidas alcohólicas</t>
   </si>
 </sst>
 </file>
@@ -449,127 +467,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>155</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>500</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>535</v>
-      </c>
-      <c r="C6" s="2">
-        <v>600</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>355</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1400</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2">
-        <v>406</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1500</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix data producto_id and inventario_id in generate report
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Producto" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Inventario" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -19,49 +19,19 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>Cerveza Artesanal Actualizada</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN</t>
-  </si>
-  <si>
-    <t>Cerveza artesanal de alta calidad, edición limitada</t>
-  </si>
-  <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>Artesanal Premium</t>
-  </si>
-  <si>
-    <t>CONTENIDO</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>UNIDAD DE MEDIDA</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>TIPO</t>
-  </si>
-  <si>
-    <t>bebida</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>1800</t>
-  </si>
-  <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
-    <t>Bebidas alcohólicas</t>
+    <t>asdfsdfs</t>
+  </si>
+  <si>
+    <t>STOCK ACTUAL</t>
+  </si>
+  <si>
+    <t>MÁXIMO STOCK</t>
+  </si>
+  <si>
+    <t>FECHA DE ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>22/11/2024</t>
   </si>
 </sst>
 </file>
@@ -467,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -492,56 +462,24 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+      <c r="B3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create get all products for specific proveedor
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Inventario" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Proveedor" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -19,19 +20,94 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>asdfsdfs</t>
-  </si>
-  <si>
-    <t>STOCK ACTUAL</t>
-  </si>
-  <si>
-    <t>MÁXIMO STOCK</t>
-  </si>
-  <si>
-    <t>FECHA DE ACTUALIZACIÓN</t>
-  </si>
-  <si>
-    <t>22/11/2024</t>
+    <t>sadasdasdsa</t>
+  </si>
+  <si>
+    <t>RUT</t>
+  </si>
+  <si>
+    <t>19.654.321-K</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>dasder85@gmail.com</t>
+  </si>
+  <si>
+    <t>TELÉFONO</t>
+  </si>
+  <si>
+    <t>123123213</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>asdasdsaasdas</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t>MARCA</t>
+  </si>
+  <si>
+    <t>CONTENIDO</t>
+  </si>
+  <si>
+    <t>UNIDAD DE MEDIDA</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>CATEGORÍA</t>
+  </si>
+  <si>
+    <t>sdfsdfsdf</t>
+  </si>
+  <si>
+    <t>32432432423</t>
+  </si>
+  <si>
+    <t>23423423423</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>Alcohólico</t>
+  </si>
+  <si>
+    <t>234234</t>
+  </si>
+  <si>
+    <t>Vino</t>
+  </si>
+  <si>
+    <t>Hola bro</t>
+  </si>
+  <si>
+    <t>Nuevo ron nuevo</t>
+  </si>
+  <si>
+    <t>NO REGISTRADO</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>Cerveza</t>
   </si>
 </sst>
 </file>
@@ -437,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -462,24 +538,32 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -489,4 +573,96 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="8" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix proveedor screen, add table for products
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -5,14 +5,13 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Proveedor" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -20,94 +19,31 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>sadasdasdsa</t>
+    <t>Proveedor nuevo nuevo</t>
   </si>
   <si>
     <t>RUT</t>
   </si>
   <si>
-    <t>19.654.321-K</t>
+    <t>20.630.735-8</t>
   </si>
   <si>
     <t>EMAIL</t>
   </si>
   <si>
-    <t>dasder85@gmail.com</t>
+    <t>t2est@proveedorejemplo.com</t>
   </si>
   <si>
     <t>TELÉFONO</t>
   </si>
   <si>
-    <t>123123213</t>
+    <t>387654321</t>
   </si>
   <si>
     <t>DIRECCIÓN</t>
   </si>
   <si>
-    <t>asdasdsaasdas</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN</t>
-  </si>
-  <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>CONTENIDO</t>
-  </si>
-  <si>
-    <t>UNIDAD DE MEDIDA</t>
-  </si>
-  <si>
-    <t>TIPO</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>CATEGORÍA</t>
-  </si>
-  <si>
-    <t>sdfsdfsdf</t>
-  </si>
-  <si>
-    <t>32432432423</t>
-  </si>
-  <si>
-    <t>23423423423</t>
-  </si>
-  <si>
-    <t>233</t>
-  </si>
-  <si>
-    <t>ML</t>
-  </si>
-  <si>
-    <t>Alcohólico</t>
-  </si>
-  <si>
-    <t>234234</t>
-  </si>
-  <si>
-    <t>Vino</t>
-  </si>
-  <si>
-    <t>Hola bro</t>
-  </si>
-  <si>
-    <t>Nuevo ron nuevo</t>
-  </si>
-  <si>
-    <t>NO REGISTRADO</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>GR</t>
-  </si>
-  <si>
-    <t>Cerveza</t>
+    <t>Called</t>
   </si>
 </sst>
 </file>
@@ -573,96 +509,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="8" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add active or desactive user in user and perfil screen
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,46 +4,55 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Proveedor" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Usuario" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
   <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>Proveedor nuevo nuevo</t>
-  </si>
-  <si>
     <t>RUT</t>
   </si>
   <si>
-    <t>20.630.735-8</t>
+    <t>12.345.678-5</t>
   </si>
   <si>
     <t>EMAIL</t>
   </si>
   <si>
-    <t>t2est@proveedorejemplo.com</t>
-  </si>
-  <si>
-    <t>TELÉFONO</t>
-  </si>
-  <si>
-    <t>387654321</t>
-  </si>
-  <si>
-    <t>DIRECCIÓN</t>
-  </si>
-  <si>
-    <t>Called</t>
+    <t>ialeczander@gmail.com</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>NOMBRE COMPLETO</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>FECHA DE REGISTRO</t>
+  </si>
+  <si>
+    <t>22/12/2024</t>
+  </si>
+  <si>
+    <t>ÚLTIMA ACTUALIZACIÓN</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -449,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -502,6 +511,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
add new attribute return in token jwt
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>CARACTERISTICAS GENERALES</t>
   </si>
@@ -25,16 +25,22 @@
     <t>RUT</t>
   </si>
   <si>
-    <t>No registrada</t>
+    <t>20.630.735-8</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>No registrado</t>
+  </si>
+  <si>
+    <t>TELÉFONO</t>
   </si>
   <si>
     <t>EMAIL</t>
   </si>
   <si>
-    <t>TELÉFONO</t>
-  </si>
-  <si>
-    <t>DIRECCIÓN</t>
+    <t>ialeczander@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -474,23 +480,23 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug with automatic update cantidad
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,43 +4,76 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Proveedor" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>CARACTERISTICAS GENERALES</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
+  <si>
+    <t>NÚMERO</t>
+  </si>
+  <si>
+    <t>FECHA DEL PEDIDO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CANTIDAD DE PRODUCTOS</t>
+  </si>
+  <si>
+    <t>COSTO TOTAL</t>
+  </si>
+  <si>
+    <t>PROVEEDOR</t>
+  </si>
+  <si>
+    <t>INVENTARIO</t>
+  </si>
+  <si>
+    <t>28/12/2024</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>$275</t>
   </si>
   <si>
     <t>don arturo</t>
   </si>
   <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>20.630.735-8</t>
-  </si>
-  <si>
-    <t>DIRECCIÓN</t>
-  </si>
-  <si>
-    <t>No registrado</t>
-  </si>
-  <si>
-    <t>TELÉFONO</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>ialeczander@gmail.com</t>
+    <t>Proveedor Ejemplotest</t>
+  </si>
+  <si>
+    <t>30/12/2024</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>Ale 123asddddddddddddddddddd</t>
+  </si>
+  <si>
+    <t>31/12/2024</t>
+  </si>
+  <si>
+    <t>$2775</t>
+  </si>
+  <si>
+    <t>$5550</t>
+  </si>
+  <si>
+    <t>$250</t>
+  </si>
+  <si>
+    <t>$333000</t>
+  </si>
+  <si>
+    <t>$100000</t>
   </si>
 </sst>
 </file>
@@ -446,63 +479,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G17"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>555</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>600</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3">
+        <v>500</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
add validation for user
</commit_message>
<xml_diff>
--- a/backend/src/tmp/exported_data.xlsx
+++ b/backend/src/tmp/exported_data.xlsx
@@ -4,59 +4,139 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Pedido" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Productos" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="Datos Exportados" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>CARACTERISTICAS GENERALES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="42">
   <si>
     <t>NÚMERO</t>
   </si>
   <si>
-    <t>ESTADO ACTUAL</t>
+    <t>FECHA DEL PEDIDO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CANTIDAD DE PRODUCTOS</t>
+  </si>
+  <si>
+    <t>COSTO TOTAL</t>
+  </si>
+  <si>
+    <t>PROVEEDOR</t>
+  </si>
+  <si>
+    <t>INVENTARIO</t>
+  </si>
+  <si>
+    <t>28/12/2024</t>
   </si>
   <si>
     <t>Completo</t>
   </si>
   <si>
-    <t>FECHA DEL PEDIDO</t>
+    <t>$275</t>
+  </si>
+  <si>
+    <t>don arturo</t>
+  </si>
+  <si>
+    <t>Proveedor Ejemplotest</t>
+  </si>
+  <si>
+    <t>30/12/2024</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>Ale 123asddddddddddddddddddd</t>
   </si>
   <si>
     <t>31/12/2024</t>
   </si>
   <si>
-    <t>TOTAL DEL PEDIDO</t>
-  </si>
-  <si>
     <t>$2775</t>
   </si>
   <si>
-    <t>NOMBRE DEL PRODUCTO</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>PRECIO</t>
-  </si>
-  <si>
-    <t>SUBTOTAL</t>
-  </si>
-  <si>
-    <t>Ale 23e</t>
-  </si>
-  <si>
-    <t>555</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>$5550</t>
+  </si>
+  <si>
+    <t>$250</t>
+  </si>
+  <si>
+    <t>$333000</t>
+  </si>
+  <si>
+    <t>$100000</t>
+  </si>
+  <si>
+    <t>01/09/2024</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>$100500</t>
+  </si>
+  <si>
+    <t>$60</t>
+  </si>
+  <si>
+    <t>19/12/2024</t>
+  </si>
+  <si>
+    <t>$16</t>
+  </si>
+  <si>
+    <t>02/01/2025</t>
+  </si>
+  <si>
+    <t>$50</t>
+  </si>
+  <si>
+    <t>Patio Trasero</t>
+  </si>
+  <si>
+    <t>$222000</t>
+  </si>
+  <si>
+    <t>$30525</t>
+  </si>
+  <si>
+    <t>$30555525</t>
+  </si>
+  <si>
+    <t>$305525</t>
+  </si>
+  <si>
+    <t>$28860</t>
+  </si>
+  <si>
+    <t>$5111106</t>
+  </si>
+  <si>
+    <t>$288860</t>
+  </si>
+  <si>
+    <t>$1265</t>
+  </si>
+  <si>
+    <t>$110055</t>
+  </si>
+  <si>
+    <t>$5100000</t>
+  </si>
+  <si>
+    <t>$101000</t>
+  </si>
+  <si>
+    <t>$200000</t>
   </si>
 </sst>
 </file>
@@ -462,94 +542,1097 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:G47"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>555</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="4" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2775</v>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>600</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3">
+        <v>500</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2">
+        <v>201</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <v>201</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3">
+        <v>400</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2">
+        <v>5</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3">
+        <v>555</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2">
+        <v>555555</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5555</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2">
+        <v>555</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3">
+        <v>232323</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5555</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="3">
+        <v>23</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2001</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="3">
+        <v>201</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="2">
+        <v>10200</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>37</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="3">
+        <v>10200</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="2">
+        <v>10200</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>39</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="3">
+        <v>10200</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="2">
+        <v>10200</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>41</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3">
+        <v>10200</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="2">
+        <v>10200</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>43</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="3">
+        <v>202</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>44</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="2">
+        <v>202</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>45</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="3">
+        <v>202</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="2">
+        <v>400</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>47</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="3">
+        <v>400</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>